<commit_message>
fix Maggie, skill engine and health engine bug
</commit_message>
<xml_diff>
--- a/Sound/music inspiration.xlsx
+++ b/Sound/music inspiration.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093ADB17-596D-4E84-8DD2-D926789AD714}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A8F4273-5696-4A33-A04D-3F188FA087DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="144">
   <si>
     <t>teseract</t>
   </si>
@@ -446,6 +447,12 @@
   </si>
   <si>
     <t>Test Hugo\2_pousse en douceur la pile de papier.wav</t>
+  </si>
+  <si>
+    <t>Ni</t>
+  </si>
+  <si>
+    <t>underground                                                                      /  city</t>
   </si>
 </sst>
 </file>
@@ -848,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,6 +1456,17 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>